<commit_message>
adding pizza items, buffing panama and bowler
</commit_message>
<xml_diff>
--- a/src/data/pizzabox-and-boosts.xlsx
+++ b/src/data/pizzabox-and-boosts.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekes\Documents\GitHub\pizzatales\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\pizzat\pizzatales\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -128,9 +128,6 @@
     <t>chicago</t>
   </si>
   <si>
-    <t>top hat</t>
-  </si>
-  <si>
     <t>rocket launcher</t>
   </si>
   <si>
@@ -144,12 +141,15 @@
   </si>
   <si>
     <t>panama</t>
+  </si>
+  <si>
+    <t>top</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -507,20 +507,20 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -539,15 +539,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -555,7 +555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -563,7 +563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -571,7 +571,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -579,7 +579,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -587,7 +587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -595,7 +595,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -603,7 +603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -611,15 +611,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -627,47 +627,47 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -675,7 +675,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -683,7 +683,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
putting boosts around maps
</commit_message>
<xml_diff>
--- a/src/data/pizzabox-and-boosts.xlsx
+++ b/src/data/pizzabox-and-boosts.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\Desktop\pizzat\pizzatales\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lekes\Documents\GitHub\pizzatales\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Level</t>
   </si>
@@ -144,12 +144,24 @@
   </si>
   <si>
     <t>top</t>
+  </si>
+  <si>
+    <t>basil</t>
+  </si>
+  <si>
+    <t>cheese armor</t>
+  </si>
+  <si>
+    <t>bacon</t>
+  </si>
+  <si>
+    <t>garlic bread</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -507,20 +519,21 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,7 +544,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -539,7 +552,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -547,7 +560,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -555,15 +568,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -571,7 +587,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -579,7 +595,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -587,15 +603,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -603,7 +622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -611,7 +630,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -619,15 +638,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -635,7 +657,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -643,7 +665,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -651,15 +673,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -667,7 +692,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -675,7 +700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -683,7 +708,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>

</xml_diff>